<commit_message>
Set correct ou and year cells
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_2.xlsx
+++ b/templates/NHWA_Module_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garza/dev/eyeseetea/WHO/excel-data-import-app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17652906-196B-0048-9AD5-5F4CD9803CF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047D4DB6-2367-C744-8FAC-FBC33D300C54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" tabRatio="391" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2697,6 +2697,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -2728,10 +2732,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2829,11 +2829,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$R$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$R$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$S$9" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$S$9" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2841,11 +2841,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$R$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$R$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$S$10" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$S$10" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2861,7 +2861,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$S$11" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$S$11" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2873,7 +2873,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$S$12" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$S$12" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2885,7 +2885,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$S$13" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$S$13" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2897,7 +2897,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$S$14" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$S$14" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2934,64 +2934,124 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>711200</xdr:colOff>
-          <xdr:row>2</xdr:row>
-          <xdr:rowOff>279400</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>3</xdr:col>
-          <xdr:colOff>12700</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>38100</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2050" name="ComboBox1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2050"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2050" name="ComboBox1" hidden="1">
+          <a:extLst>
+            <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+              <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s2050"/>
+            </a:ext>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:noFill/>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="ComboBox1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr preferRelativeResize="0">
+          <a:picLocks noChangeArrowheads="1" noChangeShapeType="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="863600"/>
+          <a:ext cx="4203700" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:noFill/>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4021,7 +4081,7 @@
                   <a14:compatExt spid="_x0000_s1179"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04C80461-F9A8-5F4A-B093-5165AED65040}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4067,14 +4127,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1180" name="Check Box 156" hidden="1">
@@ -4083,7 +4148,7 @@
                   <a14:compatExt spid="_x0000_s1180"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E71C0E7A-C295-F243-B56A-A2CFCC0A73B5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4123,20 +4188,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1181" name="Check Box 157" hidden="1">
@@ -4145,7 +4215,7 @@
                   <a14:compatExt spid="_x0000_s1181"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA9ECAB-D8A4-FF41-ACAA-5EF03F3F5DFF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4185,20 +4255,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1182" name="Check Box 158" hidden="1">
@@ -4207,7 +4282,7 @@
                   <a14:compatExt spid="_x0000_s1182"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21811C68-DE93-A94F-BB0F-A402F1F57F55}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4247,20 +4322,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1183" name="Check Box 159" hidden="1">
@@ -4269,7 +4349,7 @@
                   <a14:compatExt spid="_x0000_s1183"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA3BE3E1-6B2B-9A43-8C6B-074D20949A44}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00009F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4309,20 +4389,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1184" name="Check Box 160" hidden="1">
@@ -4331,7 +4416,7 @@
                   <a14:compatExt spid="_x0000_s1184"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97AC865B-E215-E04F-843A-9E3424B20B5E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A0040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4371,20 +4456,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1185" name="Check Box 161" hidden="1">
@@ -4393,7 +4483,7 @@
                   <a14:compatExt spid="_x0000_s1185"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{026BD36A-400F-4D40-B3E6-DF2D7F4D8619}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A1040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4433,20 +4523,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1186" name="Check Box 162" hidden="1">
@@ -4455,7 +4550,7 @@
                   <a14:compatExt spid="_x0000_s1186"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF12A74A-CA5D-3A46-AF24-1982498488DD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A2040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4495,20 +4590,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1187" name="Check Box 163" hidden="1">
@@ -4517,7 +4617,7 @@
                   <a14:compatExt spid="_x0000_s1187"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{243A2CED-728F-C245-B794-5AC82343017B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A3040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4557,20 +4657,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1188" name="Check Box 164" hidden="1">
@@ -4579,7 +4684,7 @@
                   <a14:compatExt spid="_x0000_s1188"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9AAC0EE-B98B-C346-860A-0422363D4755}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A4040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4619,20 +4724,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1189" name="Check Box 165" hidden="1">
@@ -4641,7 +4751,7 @@
                   <a14:compatExt spid="_x0000_s1189"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1825D472-A9C9-FC48-B2DE-AE57943BB051}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A5040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4681,20 +4791,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1190" name="Check Box 166" hidden="1">
@@ -4703,7 +4818,7 @@
                   <a14:compatExt spid="_x0000_s1190"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1C4B398-6048-1845-9A59-5FEEAE3AE926}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A6040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4743,20 +4858,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1191" name="Check Box 167" hidden="1">
@@ -4765,7 +4885,7 @@
                   <a14:compatExt spid="_x0000_s1191"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAB99A1B-C4B7-D24B-9EDC-2AA3AEBBAC5B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A7040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4805,20 +4925,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1192" name="Check Box 168" hidden="1">
@@ -4827,7 +4952,7 @@
                   <a14:compatExt spid="_x0000_s1192"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA19133C-AD1B-374C-900C-6FF58EA49130}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A8040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4867,20 +4992,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1193" name="Check Box 169" hidden="1">
@@ -4889,7 +5019,7 @@
                   <a14:compatExt spid="_x0000_s1193"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB585550-6282-4C4E-A07E-7AB56325536D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000A9040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4929,20 +5059,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1194" name="Check Box 170" hidden="1">
@@ -4951,7 +5086,7 @@
                   <a14:compatExt spid="_x0000_s1194"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48D97120-61FD-6D44-BBD0-C5106F96FC42}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AA040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4991,20 +5126,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1195" name="Check Box 171" hidden="1">
@@ -5013,7 +5153,7 @@
                   <a14:compatExt spid="_x0000_s1195"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E99E8E83-CBDE-FC46-ABC2-7328AE2E5493}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AB040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5053,20 +5193,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1196" name="Check Box 172" hidden="1">
@@ -5075,7 +5220,7 @@
                   <a14:compatExt spid="_x0000_s1196"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2521BA91-2741-F24E-A384-75DE767BB8F3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AC040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5115,20 +5260,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1197" name="Check Box 173" hidden="1">
@@ -5137,7 +5287,7 @@
                   <a14:compatExt spid="_x0000_s1197"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3BDE7C6-6EE0-DF42-A9DF-7CE43C53880E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AD040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5177,20 +5327,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1198" name="Check Box 174" hidden="1">
@@ -5199,7 +5354,7 @@
                   <a14:compatExt spid="_x0000_s1198"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD2C00D7-E331-8243-A181-1D1C729C9F5B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AE040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5239,20 +5394,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1199" name="Check Box 175" hidden="1">
@@ -5261,7 +5421,7 @@
                   <a14:compatExt spid="_x0000_s1199"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A0E8FBF-AFBF-8F4D-829E-22D292A79B21}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000AF040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5301,20 +5461,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1200" name="Check Box 176" hidden="1">
@@ -5323,7 +5488,7 @@
                   <a14:compatExt spid="_x0000_s1200"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C93F68C-1CC8-2944-86B9-0A062CEF8CA3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B0040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5363,20 +5528,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1201" name="Check Box 177" hidden="1">
@@ -5385,7 +5555,7 @@
                   <a14:compatExt spid="_x0000_s1201"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9850C065-D05E-C54F-A919-4C1BF3668766}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B1040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5425,20 +5595,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1202" name="Check Box 178" hidden="1">
@@ -5447,7 +5622,7 @@
                   <a14:compatExt spid="_x0000_s1202"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CF7FADA-0CDC-D24F-BCDD-4B85E5C56C2D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B2040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5487,20 +5662,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1204" name="Check Box 180" hidden="1">
@@ -5509,7 +5689,7 @@
                   <a14:compatExt spid="_x0000_s1204"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4934894E-86AA-C243-92A9-B662463092EB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B4040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5549,20 +5729,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>685800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>101600</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="698500" cy="177800"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>1384300</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>279400</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1206" name="Check Box 182" hidden="1">
@@ -5571,7 +5756,7 @@
                   <a14:compatExt spid="_x0000_s1206"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A22D429F-B328-F144-AB03-BAA6D8839C13}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000B6040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5611,7 +5796,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -5938,7 +6123,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BZ250"/>
   <sheetViews>
@@ -5970,20 +6155,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -6010,20 +6195,20 @@
       </c>
     </row>
     <row r="2" spans="2:31" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>777</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -6195,27 +6380,27 @@
       </c>
     </row>
     <row r="6" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="37" t="s">
         <v>770</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="37" t="s">
         <v>771</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="37" t="s">
         <v>772</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37" t="s">
+      <c r="F6" s="37"/>
+      <c r="G6" s="38" t="s">
         <v>773</v>
       </c>
-      <c r="H6" s="36" t="s">
+      <c r="H6" s="37" t="s">
         <v>774</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36" t="s">
+      <c r="I6" s="37"/>
+      <c r="J6" s="37" t="s">
         <v>775</v>
       </c>
       <c r="K6" s="26" t="s">
@@ -6224,11 +6409,11 @@
       <c r="L6" s="26"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35"/>
-      <c r="S6" s="35"/>
-      <c r="T6" s="35"/>
+      <c r="P6" s="36"/>
+      <c r="Q6" s="36"/>
+      <c r="R6" s="36"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
       <c r="Y6" s="7" t="s">
         <v>19</v>
       </c>
@@ -6255,23 +6440,23 @@
       </c>
     </row>
     <row r="7" spans="2:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="37"/>
+      <c r="G7" s="38"/>
       <c r="H7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="36"/>
+      <c r="J7" s="37"/>
       <c r="K7" s="20" t="s">
         <v>12</v>
       </c>
@@ -12828,7 +13013,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -12858,36 +13042,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
     </row>
     <row r="2" spans="2:14" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>777</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
       <c r="N2" s="17" t="e">
         <f>Input!V2</f>
         <v>#N/A</v>
@@ -12940,26 +13124,26 @@
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="40" t="s">
         <v>768</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="37" t="s">
         <v>769</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="37"/>
       <c r="L6" s="8"/>
       <c r="N6" s="17" t="s">
         <v>788</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
       <c r="L7" s="8"/>
       <c r="N7" s="17"/>
     </row>
@@ -12970,8 +13154,8 @@
       <c r="C8" s="11" t="s">
         <v>786</v>
       </c>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="39"/>
       <c r="L8" s="8"/>
       <c r="N8" s="17">
         <v>1</v>
@@ -12985,41 +13169,41 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="37" t="s">
         <v>770</v>
       </c>
-      <c r="D10" s="36" t="s">
+      <c r="D10" s="37" t="s">
         <v>778</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="38" t="s">
         <v>779</v>
       </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37" t="s">
+      <c r="F10" s="38"/>
+      <c r="G10" s="38" t="s">
         <v>780</v>
       </c>
-      <c r="H10" s="37"/>
-      <c r="I10" s="37" t="s">
+      <c r="H10" s="38"/>
+      <c r="I10" s="38" t="s">
         <v>795</v>
       </c>
-      <c r="J10" s="37" t="s">
+      <c r="J10" s="38" t="s">
         <v>783</v>
       </c>
-      <c r="K10" s="37" t="s">
+      <c r="K10" s="38" t="s">
         <v>784</v>
       </c>
-      <c r="L10" s="37" t="s">
+      <c r="L10" s="38" t="s">
         <v>785</v>
       </c>
       <c r="N10" s="17"/>
     </row>
     <row r="11" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
       <c r="E11" s="19" t="s">
         <v>12</v>
       </c>
@@ -13032,10 +13216,10 @@
       <c r="H11" s="19" t="s">
         <v>782</v>
       </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
     </row>
     <row r="12" spans="2:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="10">
@@ -13214,8 +13398,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13230,22 +13414,21 @@
     <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
     <col min="10" max="12" width="16.5" style="1" customWidth="1"/>
     <col min="13" max="14" width="18.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="20" width="9.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="43" width="9.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" style="1" customWidth="1"/>
+    <col min="16" max="43" width="9.1640625" style="1" customWidth="1"/>
     <col min="44" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -13255,15 +13438,15 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="2:28" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="35" t="s">
         <v>791</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -13332,18 +13515,18 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
       <c r="H6" s="33"/>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
@@ -13354,8 +13537,8 @@
       <c r="O6" s="33"/>
     </row>
     <row r="7" spans="2:28" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="41"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="31" t="s">
         <v>789</v>
       </c>
@@ -13427,7 +13610,7 @@
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="32"/>
-      <c r="F9" s="44"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="32"/>
       <c r="H9" s="33"/>
       <c r="I9" s="33"/>
@@ -13444,10 +13627,10 @@
         <v>0</v>
       </c>
       <c r="R9" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T9" s="17"/>
       <c r="U9" s="17"/>
@@ -13468,7 +13651,7 @@
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="32"/>
-      <c r="F10" s="44"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="32"/>
       <c r="H10" s="33"/>
       <c r="I10" s="33"/>
@@ -13485,10 +13668,10 @@
         <v>0</v>
       </c>
       <c r="R10" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T10" s="17"/>
       <c r="U10" s="17"/>
@@ -13509,7 +13692,7 @@
       </c>
       <c r="D11" s="32"/>
       <c r="E11" s="32"/>
-      <c r="F11" s="44"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="32"/>
       <c r="H11" s="33"/>
       <c r="I11" s="33"/>
@@ -13529,7 +13712,7 @@
         <v>0</v>
       </c>
       <c r="S11" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T11" s="17"/>
       <c r="U11" s="17"/>
@@ -13550,7 +13733,7 @@
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="32"/>
-      <c r="F12" s="44"/>
+      <c r="F12" s="34"/>
       <c r="G12" s="32"/>
       <c r="H12" s="33"/>
       <c r="I12" s="33"/>
@@ -13570,7 +13753,7 @@
         <v>0</v>
       </c>
       <c r="S12" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="17"/>
       <c r="U12" s="17"/>
@@ -13591,7 +13774,7 @@
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="32"/>
-      <c r="F13" s="44"/>
+      <c r="F13" s="34"/>
       <c r="G13" s="32"/>
       <c r="H13" s="33"/>
       <c r="I13" s="33"/>
@@ -13611,7 +13794,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T13" s="17"/>
       <c r="U13" s="17"/>
@@ -13632,7 +13815,7 @@
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="32"/>
-      <c r="F14" s="44"/>
+      <c r="F14" s="34"/>
       <c r="G14" s="32"/>
       <c r="H14" s="33"/>
       <c r="I14" s="33"/>
@@ -13652,7 +13835,7 @@
         <v>0</v>
       </c>
       <c r="S14" s="17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T14" s="17"/>
       <c r="U14" s="17"/>

</xml_diff>

<commit_message>
Hide checkbox value cols and add whole number validations
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_2.xlsx
+++ b/templates/NHWA_Module_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garza/dev/eyeseetea/WHO/excel-data-import-app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{047D4DB6-2367-C744-8FAC-FBC33D300C54}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EAA996-35E0-CB4F-8818-4AF5AB872BFC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" tabRatio="391" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6128,7 +6128,7 @@
   <dimension ref="A1:BZ250"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="D8" sqref="D8:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13010,6 +13010,11 @@
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="J6:J7"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:L14" xr:uid="{33779F28-38A2-1441-9C08-B723497EF83A}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -13022,7 +13027,7 @@
   <dimension ref="B1:N18"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="D12" sqref="D12:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13358,6 +13363,11 @@
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="J10:J11"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:L18" xr:uid="{F5DF63A6-AF5F-234E-93B2-CD779E2D35B1}">
+      <formula1>0</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -13398,8 +13408,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13414,8 +13424,9 @@
     <col min="9" max="9" width="18.5" style="1" customWidth="1"/>
     <col min="10" max="12" width="16.5" style="1" customWidth="1"/>
     <col min="13" max="14" width="18.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.5" style="1" customWidth="1"/>
-    <col min="16" max="43" width="9.1640625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="20" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="43" width="9.1640625" style="1" customWidth="1"/>
     <col min="44" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Apply form changes to module 2 template and script
</commit_message>
<xml_diff>
--- a/templates/NHWA_Module_2.xlsx
+++ b/templates/NHWA_Module_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Garza/dev/eyeseetea/WHO/excel-data-import-app/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EAA996-35E0-CB4F-8818-4AF5AB872BFC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83218C29-53C2-2D49-A259-4C693B78DD21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" tabRatio="391" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="14100" tabRatio="391" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="796">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="799">
   <si>
     <t xml:space="preserve">NATIONAL  HEALTH WORKFORCE ACCOUNTS DATA </t>
   </si>
@@ -2347,30 +2347,9 @@
     <t>HWF Education and Training Programme</t>
   </si>
   <si>
-    <t>Applications</t>
-  </si>
-  <si>
-    <t>Applications By Gender</t>
-  </si>
-  <si>
-    <t>Admissions</t>
-  </si>
-  <si>
-    <t>Admissions By Gender</t>
-  </si>
-  <si>
-    <t>Entrants</t>
-  </si>
-  <si>
-    <t>Entrants By Gender</t>
-  </si>
-  <si>
     <t>Health Workforce Education and Training</t>
   </si>
   <si>
-    <t>Graduates</t>
-  </si>
-  <si>
     <t>Graduates By Gender</t>
   </si>
   <si>
@@ -2419,7 +2398,37 @@
     <t>Other Databases</t>
   </si>
   <si>
-    <t>Students Quitting</t>
+    <t>Applications (2-03)</t>
+  </si>
+  <si>
+    <t>Applications By Gender (2-03)</t>
+  </si>
+  <si>
+    <t>Admissions (2-04)</t>
+  </si>
+  <si>
+    <t>Admissions By Gender (2-04)</t>
+  </si>
+  <si>
+    <t>Enrolled (2-05)</t>
+  </si>
+  <si>
+    <t>Enrolled By Gender (2-05)</t>
+  </si>
+  <si>
+    <t>Graduates (2-07)</t>
+  </si>
+  <si>
+    <t>Drop-outs (number) (2-06)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>PARTIAL</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -2511,7 +2520,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2576,12 +2585,27 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
-      </left>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
-      <top/>
-      <bottom/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -2608,7 +2632,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2672,9 +2696,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2705,6 +2726,13 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2714,24 +2742,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -2769,7 +2819,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$N$8" fmlaRange="$N$4:$N$6" noThreeD="1" sel="1" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="16" fmlaLink="$P$8" fmlaRange="$P$4:$P$7" noThreeD="1" sel="1" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3067,8 +3117,8 @@
           <xdr:rowOff>12700</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>1066800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -6128,7 +6178,7 @@
   <dimension ref="A1:BZ250"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:L14"/>
+      <selection activeCell="U1" sqref="U1:AH1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6136,39 +6186,42 @@
     <col min="1" max="1" width="9.1640625" style="7"/>
     <col min="2" max="2" width="10.83203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="53.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="13.1640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="7" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="7" customWidth="1"/>
     <col min="7" max="7" width="12.1640625" style="7" customWidth="1"/>
     <col min="8" max="8" width="10.1640625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="10" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.33203125" style="7" customWidth="1"/>
-    <col min="11" max="15" width="9.1640625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="7" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" style="7" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="7" customWidth="1"/>
+    <col min="13" max="15" width="9.1640625" style="7" customWidth="1"/>
     <col min="16" max="16" width="12.5" style="7" customWidth="1"/>
     <col min="17" max="17" width="11.5" style="7" customWidth="1"/>
     <col min="18" max="18" width="16.33203125" style="7" customWidth="1"/>
     <col min="19" max="19" width="12" style="7" customWidth="1"/>
     <col min="20" max="20" width="12.1640625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="9.6640625" style="7" customWidth="1"/>
-    <col min="22" max="33" width="9.1640625" style="7" customWidth="1"/>
-    <col min="34" max="16384" width="9.1640625" style="7"/>
+    <col min="21" max="21" width="9.6640625" style="7" hidden="1" customWidth="1"/>
+    <col min="22" max="33" width="9.1640625" style="7" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:31" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
@@ -6177,7 +6230,7 @@
       <c r="T1" s="3"/>
       <c r="U1" s="3"/>
       <c r="V1" s="15" t="s">
-        <v>792</v>
+        <v>785</v>
       </c>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
@@ -6195,20 +6248,20 @@
       </c>
     </row>
     <row r="2" spans="2:31" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>777</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
+      <c r="B2" s="36" t="s">
+        <v>771</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
@@ -6379,41 +6432,41 @@
         <v>Botswana</v>
       </c>
     </row>
-    <row r="6" spans="2:31" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+    <row r="6" spans="2:31" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="38" t="s">
         <v>770</v>
       </c>
-      <c r="D6" s="37" t="s">
-        <v>771</v>
-      </c>
-      <c r="E6" s="37" t="s">
-        <v>772</v>
-      </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38" t="s">
-        <v>773</v>
-      </c>
-      <c r="H6" s="37" t="s">
-        <v>774</v>
-      </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37" t="s">
-        <v>775</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>776</v>
-      </c>
-      <c r="L6" s="26"/>
+      <c r="D6" s="38" t="s">
+        <v>788</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>789</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39" t="s">
+        <v>790</v>
+      </c>
+      <c r="H6" s="38" t="s">
+        <v>791</v>
+      </c>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38" t="s">
+        <v>792</v>
+      </c>
+      <c r="K6" s="40" t="s">
+        <v>793</v>
+      </c>
+      <c r="L6" s="41"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
       <c r="Y6" s="7" t="s">
         <v>19</v>
       </c>
@@ -6439,24 +6492,24 @@
         <v>Burkina Faso</v>
       </c>
     </row>
-    <row r="7" spans="2:31" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
+    <row r="7" spans="2:31" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
       <c r="E7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="38"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="20" t="s">
         <v>12</v>
       </c>
       <c r="I7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="37"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="20" t="s">
         <v>12</v>
       </c>
@@ -12997,7 +13050,7 @@
   <protectedRanges>
     <protectedRange sqref="L4 Q8:R15 D8:D11 D13:D14 E8:L14 N8:P14" name="Range1"/>
   </protectedRanges>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="B1:M1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="S6:T6"/>
@@ -13009,6 +13062,7 @@
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="J6:J7"/>
+    <mergeCell ref="K6:L6"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:L14" xr:uid="{33779F28-38A2-1441-9C08-B723497EF83A}">
@@ -13024,10 +13078,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B1:N18"/>
+  <dimension ref="B1:T18"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13035,54 +13089,59 @@
     <col min="1" max="1" width="9.1640625" style="7"/>
     <col min="2" max="2" width="10.83203125" style="7" customWidth="1"/>
     <col min="3" max="3" width="53.5" style="7" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="7" customWidth="1"/>
-    <col min="5" max="7" width="11" style="7" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="7" customWidth="1"/>
+    <col min="6" max="7" width="11" style="7" customWidth="1"/>
     <col min="8" max="9" width="9.6640625" style="7" customWidth="1"/>
     <col min="10" max="10" width="10" style="7" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="7" customWidth="1"/>
     <col min="12" max="12" width="9.83203125" style="7" customWidth="1"/>
     <col min="13" max="13" width="8.83203125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="9.1640625" style="7" hidden="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1640625" style="7"/>
+    <col min="14" max="14" width="9.1640625" style="7" customWidth="1"/>
+    <col min="15" max="15" width="9.1640625" style="7"/>
+    <col min="16" max="20" width="0" style="7" hidden="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1640625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="35" t="s">
+    <row r="1" spans="2:20" ht="23" x14ac:dyDescent="0.2">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-    </row>
-    <row r="2" spans="2:14" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>777</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="17" t="e">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+    </row>
+    <row r="2" spans="2:20" ht="23" x14ac:dyDescent="0.2">
+      <c r="B2" s="36" t="s">
+        <v>771</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="17" t="e">
         <f>Input!V2</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="2:14" ht="23" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:20" ht="23" x14ac:dyDescent="0.2">
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -13095,9 +13154,11 @@
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
-      <c r="N3" s="17"/>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
@@ -13119,96 +13180,123 @@
         <f>Input!L4</f>
         <v>0</v>
       </c>
-      <c r="N4" s="17"/>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P4" s="17"/>
+    </row>
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B5" s="8"/>
       <c r="L5" s="8"/>
-      <c r="N5" s="17" t="s">
-        <v>787</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+      <c r="P5" s="17" t="s">
+        <v>780</v>
+      </c>
+      <c r="R5" s="7" t="s">
+        <v>780</v>
+      </c>
+      <c r="S5" s="7" t="s">
+        <v>797</v>
+      </c>
+      <c r="T5" s="7" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="46" t="s">
         <v>768</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="38" t="s">
         <v>769</v>
       </c>
-      <c r="E6" s="37"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38" t="s">
+        <v>798</v>
+      </c>
       <c r="L6" s="8"/>
-      <c r="N6" s="17" t="s">
-        <v>788</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="37"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
+      <c r="P6" s="17" t="s">
+        <v>797</v>
+      </c>
+      <c r="R6" s="7" t="str">
+        <f>IF($P$8=2, "True", "")</f>
+        <v/>
+      </c>
+      <c r="S6" s="7" t="str">
+        <f>IF($P$8=3, "True", "")</f>
+        <v/>
+      </c>
+      <c r="T6" s="7" t="str">
+        <f>IF($P$8=4, "True", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
       <c r="L7" s="8"/>
-      <c r="N7" s="17"/>
-    </row>
-    <row r="8" spans="2:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="B8" s="27">
-        <v>1</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>786</v>
-      </c>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
+      <c r="P7" s="17" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="53" t="s">
+        <v>779</v>
+      </c>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="52"/>
       <c r="L8" s="8"/>
-      <c r="N8" s="17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P8" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L9" s="8"/>
-      <c r="N9" s="17" t="str">
-        <f>IF(N8=2,"true",IF(N8=3,"false",""))</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="37" t="s">
+      <c r="P9" s="17"/>
+    </row>
+    <row r="10" spans="2:20" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="38" t="s">
         <v>770</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="38" t="s">
+        <v>794</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>772</v>
+      </c>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39" t="s">
+        <v>773</v>
+      </c>
+      <c r="H10" s="39"/>
+      <c r="I10" s="43" t="s">
+        <v>795</v>
+      </c>
+      <c r="J10" s="44"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="39" t="s">
+        <v>776</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>777</v>
+      </c>
+      <c r="N10" s="39" t="s">
         <v>778</v>
       </c>
-      <c r="E10" s="38" t="s">
-        <v>779</v>
-      </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38" t="s">
-        <v>780</v>
-      </c>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38" t="s">
-        <v>795</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>783</v>
-      </c>
-      <c r="K10" s="38" t="s">
-        <v>784</v>
-      </c>
-      <c r="L10" s="38" t="s">
-        <v>785</v>
-      </c>
-      <c r="N10" s="17"/>
-    </row>
-    <row r="11" spans="2:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
+      <c r="P10" s="17"/>
+    </row>
+    <row r="11" spans="2:20" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="19" t="s">
         <v>12</v>
       </c>
@@ -13216,17 +13304,25 @@
         <v>13</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>781</v>
+        <v>774</v>
       </c>
       <c r="H11" s="19" t="s">
-        <v>782</v>
-      </c>
-      <c r="I11" s="38"/>
-      <c r="J11" s="38"/>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-    </row>
-    <row r="12" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+        <v>775</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>796</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="L11" s="39"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="39"/>
+    </row>
+    <row r="12" spans="2:20" ht="16" x14ac:dyDescent="0.2">
       <c r="B12" s="10">
         <v>1</v>
       </c>
@@ -13242,8 +13338,10 @@
       <c r="J12" s="13"/>
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
-    </row>
-    <row r="13" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+    </row>
+    <row r="13" spans="2:20" ht="16" x14ac:dyDescent="0.2">
       <c r="B13" s="10">
         <v>2</v>
       </c>
@@ -13259,8 +13357,10 @@
       <c r="J13" s="13"/>
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
-    </row>
-    <row r="14" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="2:20" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="10">
         <v>3</v>
       </c>
@@ -13276,8 +13376,10 @@
       <c r="J14" s="13"/>
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
-    </row>
-    <row r="15" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+    </row>
+    <row r="15" spans="2:20" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="10">
         <v>4</v>
       </c>
@@ -13293,8 +13395,10 @@
       <c r="J15" s="13"/>
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
-    </row>
-    <row r="16" spans="2:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+    </row>
+    <row r="16" spans="2:20" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="10">
         <v>5</v>
       </c>
@@ -13310,8 +13414,10 @@
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
-    </row>
-    <row r="17" spans="2:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+    </row>
+    <row r="17" spans="2:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="10">
         <v>6</v>
       </c>
@@ -13327,8 +13433,10 @@
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-    </row>
-    <row r="18" spans="2:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+    </row>
+    <row r="18" spans="2:14" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="10">
         <v>7</v>
       </c>
@@ -13344,11 +13452,13 @@
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
+  <mergeCells count="16">
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
@@ -13357,14 +13467,15 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:E7"/>
+    <mergeCell ref="F6:F7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="I10:K10"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:L18" xr:uid="{F5DF63A6-AF5F-234E-93B2-CD779E2D35B1}">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:N18" xr:uid="{F5DF63A6-AF5F-234E-93B2-CD779E2D35B1}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -13387,8 +13498,8 @@
                     <xdr:rowOff>12700</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
-                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:col>4</xdr:col>
+                    <xdr:colOff>1066800</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </to>
@@ -13408,8 +13519,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:AB51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:T1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13425,21 +13536,21 @@
     <col min="10" max="12" width="16.5" style="1" customWidth="1"/>
     <col min="13" max="14" width="18.33203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.5" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="20" width="9.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="43" width="9.1640625" style="1" customWidth="1"/>
+    <col min="16" max="22" width="9.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="23" max="43" width="9.1640625" style="1" customWidth="1"/>
     <col min="44" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:28" ht="23" x14ac:dyDescent="0.2">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
@@ -13449,15 +13560,15 @@
       <c r="O1" s="3"/>
     </row>
     <row r="2" spans="2:28" ht="23" x14ac:dyDescent="0.2">
-      <c r="B2" s="35" t="s">
-        <v>791</v>
-      </c>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
+      <c r="B2" s="36" t="s">
+        <v>784</v>
+      </c>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
@@ -13526,62 +13637,62 @@
       <c r="O5" s="4"/>
     </row>
     <row r="6" spans="2:28" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="43" t="s">
+      <c r="D6" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
     </row>
     <row r="7" spans="2:28" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="41"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="31" t="s">
-        <v>789</v>
-      </c>
-      <c r="E7" s="31" t="s">
-        <v>790</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>793</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>794</v>
-      </c>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="30" t="s">
+        <v>782</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>783</v>
+      </c>
+      <c r="F7" s="30" t="s">
+        <v>786</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>787</v>
+      </c>
+      <c r="H7" s="32"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32"/>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
     </row>
     <row r="8" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="10">
         <v>1</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="32"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -13616,20 +13727,20 @@
       <c r="B9" s="10">
         <v>2</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>767</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
       <c r="O9" s="7"/>
       <c r="P9" s="17" t="b">
         <v>0</v>
@@ -13657,21 +13768,21 @@
       <c r="B10" s="10">
         <v>3</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="33"/>
-      <c r="L10" s="33"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
+      <c r="O10" s="32"/>
       <c r="P10" s="17" t="b">
         <v>0</v>
       </c>
@@ -13698,21 +13809,21 @@
       <c r="B11" s="10">
         <v>4</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="32"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="32"/>
       <c r="P11" s="17" t="b">
         <v>0</v>
       </c>
@@ -13739,21 +13850,21 @@
       <c r="B12" s="10">
         <v>5</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
-      <c r="L12" s="33"/>
-      <c r="M12" s="33"/>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
+      <c r="O12" s="32"/>
       <c r="P12" s="17" t="b">
         <v>0</v>
       </c>
@@ -13780,21 +13891,21 @@
       <c r="B13" s="10">
         <v>6</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="32"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
       <c r="P13" s="17" t="b">
         <v>0</v>
       </c>
@@ -13821,21 +13932,21 @@
       <c r="B14" s="10">
         <v>7</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="32"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
       <c r="P14" s="17" t="b">
         <v>0</v>
       </c>
@@ -13859,20 +13970,20 @@
       <c r="AB14" s="17"/>
     </row>
     <row r="15" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="28"/>
-      <c r="C15" s="29"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
-      <c r="K15" s="33"/>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
@@ -13902,8 +14013,24 @@
       <c r="M16" s="7"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P16" s="1" t="str">
+        <f>IF(P8=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="Q16" s="1" t="str">
+        <f t="shared" ref="Q16:S16" si="0">IF(Q8=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="R16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="S16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -13918,8 +14045,24 @@
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P17" s="1" t="str">
+        <f t="shared" ref="P17:S17" si="1">IF(P9=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="Q17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="R17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="S17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -13934,8 +14077,24 @@
       <c r="M18" s="7"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P18" s="1" t="str">
+        <f t="shared" ref="P18:S18" si="2">IF(P10=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="Q18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="R18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S18" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -13950,8 +14109,24 @@
       <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
-    </row>
-    <row r="20" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P19" s="1" t="str">
+        <f t="shared" ref="P19:S19" si="3">IF(P11=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="Q19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="R19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+      <c r="S19" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -13966,8 +14141,24 @@
       <c r="M20" s="7"/>
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
-    </row>
-    <row r="21" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P20" s="1" t="str">
+        <f t="shared" ref="P20:S20" si="4">IF(P12=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="Q20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="R20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="S20" s="1" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -13981,8 +14172,24 @@
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
       <c r="N21" s="7"/>
-    </row>
-    <row r="22" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P21" s="1" t="str">
+        <f t="shared" ref="P21:S21" si="5">IF(P13=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="Q21" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R21" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S21" s="1" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -13996,8 +14203,24 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
       <c r="N22" s="7"/>
-    </row>
-    <row r="23" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P22" s="1" t="str">
+        <f t="shared" ref="P22:S22" si="6">IF(P14=TRUE, "True", "")</f>
+        <v/>
+      </c>
+      <c r="Q22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="R22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="S22" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -14012,7 +14235,7 @@
       <c r="M23" s="7"/>
       <c r="N23" s="7"/>
     </row>
-    <row r="24" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -14027,7 +14250,7 @@
       <c r="M24" s="7"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -14042,7 +14265,7 @@
       <c r="M25" s="7"/>
       <c r="N25" s="7"/>
     </row>
-    <row r="26" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -14057,7 +14280,7 @@
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -14072,7 +14295,7 @@
       <c r="M27" s="7"/>
       <c r="N27" s="7"/>
     </row>
-    <row r="28" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -14087,7 +14310,7 @@
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
     </row>
-    <row r="29" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -14102,7 +14325,7 @@
       <c r="M29" s="7"/>
       <c r="N29" s="7"/>
     </row>
-    <row r="30" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -14117,7 +14340,7 @@
       <c r="M30" s="7"/>
       <c r="N30" s="7"/>
     </row>
-    <row r="31" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -14132,7 +14355,7 @@
       <c r="M31" s="7"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="2:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>

</xml_diff>